<commit_message>
Elaboracao do primeiro relatorio de status da sprint 3
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Sprint-Backlog-Sprint-03#.xlsx
+++ b/Trunk/Doc/Sprint-Backlog-Sprint-03#.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto Final\fusioness\Trunk\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="-435" windowWidth="25605" windowHeight="16005"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint-Backlog" sheetId="2" r:id="rId1"/>
     <sheet name="Burndown-Chart" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -94,9 +99,6 @@
   </si>
   <si>
     <t>Executar o caso de teste</t>
-  </si>
-  <si>
-    <t>BACKLOG DA SPRINT Nº &lt;2#&gt;</t>
   </si>
   <si>
     <t>Implementar CRUD completo (Com validação)</t>
@@ -187,6 +189,9 @@
   </si>
   <si>
     <t>Como usuário gostaria de poder qualificar uma rota que participei - Quanto ao tipo de pista (WEB)</t>
+  </si>
+  <si>
+    <t>BACKLOG DA SPRINT Nº &lt;3#&gt;</t>
   </si>
 </sst>
 </file>
@@ -493,7 +498,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -521,6 +526,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -719,6 +727,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -752,6 +768,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -779,8 +796,8 @@
               <c:idx val="9"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0231845238095238"/>
-                  <c:y val="-0.0452517853872917"/>
+                  <c:x val="-2.3184523809523801E-2"/>
+                  <c:y val="-4.5251785387291701E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -790,13 +807,18 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0201488095238095"/>
-                  <c:y val="-0.0374998474027956"/>
+                  <c:x val="-2.0148809523809499E-2"/>
+                  <c:y val="-3.7499847402795598E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -806,13 +828,18 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0186607142857143"/>
-                  <c:y val="-0.0297479094182995"/>
+                  <c:x val="-1.8660714285714301E-2"/>
+                  <c:y val="-2.9747909418299499E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -822,7 +849,19 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -845,6 +884,12 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -903,46 +948,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -989,6 +1034,13 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1013,6 +1065,12 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1071,46 +1129,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0</c:v>
+                  <c:v>-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,16 +1186,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2123332408"/>
-        <c:axId val="2123335352"/>
+        <c:axId val="6945344"/>
+        <c:axId val="6946432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123332408"/>
+        <c:axId val="6945344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1151,7 +1210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123335352"/>
+        <c:crossAx val="6946432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1159,7 +1218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123335352"/>
+        <c:axId val="6946432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,13 +1245,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123332408"/>
+        <c:crossAx val="6945344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1201,7 +1261,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.511811024" r="0.511811024" t="0.787401575" header="0.31496062" footer="0.31496062"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1529,97 +1589,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="T71" sqref="T71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="2" customWidth="1"/>
-    <col min="5" max="18" width="4.6640625" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="2" customWidth="1"/>
+    <col min="5" max="18" width="4.7109375" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1">
-      <c r="A1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="A3" s="11" t="s">
+    <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+    </row>
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1663,77 +1723,79 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="3" t="e">
-        <f>SUM(E7:E9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F5" s="3" t="e">
-        <f>SUM(F7:F9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G5" s="3" t="e">
-        <f>SUM(G7:G9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H5" s="3" t="e">
-        <f>SUM(H7:H9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I5" s="3" t="e">
-        <f>SUM(I7:I9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J5" s="3" t="e">
-        <f>SUM(J7:J9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K5" s="3" t="e">
-        <f>SUM(K7:K9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L5" s="3" t="e">
-        <f>SUM(L7:L9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M5" s="3" t="e">
-        <f>SUM(M7:M9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N5" s="3" t="e">
-        <f>SUM(N7:N9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O5" s="3" t="e">
-        <f>SUM(O7:O9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P5" s="3" t="e">
-        <f>SUM(P7:P9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q5" s="3" t="e">
-        <f>SUM(Q7:Q9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R5" s="3" t="e">
-        <f>SUM(R7:R9)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="3">
+        <f>SUM(E7:E9)+SUM(E11:E13)</f>
+        <v>20</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:R5" si="0">SUM(F7:F9)+SUM(F11:F13)</f>
+        <v>20</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="M5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="O5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="Q5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="R5" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <v>10</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1749,13 +1811,13 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="70">
+    <row r="7" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="9">
         <v>8</v>
@@ -1767,49 +1829,49 @@
         <v>8</v>
       </c>
       <c r="G7" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J7" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K7" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L7" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M7" s="9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N7" s="9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="O7" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P7" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q7" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="10">
         <v>1</v>
@@ -1845,25 +1907,25 @@
         <v>1</v>
       </c>
       <c r="O8" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="10">
         <v>1</v>
@@ -1899,24 +1961,24 @@
         <v>1</v>
       </c>
       <c r="O9" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1935,13 +1997,13 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" ht="70">
+    <row r="11" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="9">
         <v>8</v>
@@ -1968,34 +2030,34 @@
         <v>8</v>
       </c>
       <c r="L11" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M11" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N11" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O11" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P11" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q11" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="10">
         <v>1</v>
@@ -2031,25 +2093,25 @@
         <v>1</v>
       </c>
       <c r="O12" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="10">
         <v>1</v>
@@ -2085,27 +2147,29 @@
         <v>1</v>
       </c>
       <c r="O13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4">
+        <v>10</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -2121,13 +2185,13 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="70">
+    <row r="15" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="9">
         <v>8</v>
@@ -2142,46 +2206,46 @@
         <v>8</v>
       </c>
       <c r="H15" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I15" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J15" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K15" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L15" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M15" s="9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N15" s="9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="O15" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P15" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q15" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="10">
         <v>1</v>
@@ -2217,25 +2281,25 @@
         <v>1</v>
       </c>
       <c r="O16" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
@@ -2271,24 +2335,24 @@
         <v>1</v>
       </c>
       <c r="O17" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>38</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -2307,13 +2371,13 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="70">
+    <row r="19" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="9">
         <v>8</v>
@@ -2340,34 +2404,34 @@
         <v>8</v>
       </c>
       <c r="L19" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M19" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N19" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O19" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P19" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R19" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="10">
         <v>1</v>
@@ -2403,25 +2467,25 @@
         <v>1</v>
       </c>
       <c r="O20" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="10">
         <v>1</v>
@@ -2457,27 +2521,29 @@
         <v>1</v>
       </c>
       <c r="O21" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>40</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="4">
+        <v>10</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2493,13 +2559,13 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" ht="70">
+    <row r="23" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="9">
         <v>8</v>
@@ -2526,34 +2592,34 @@
         <v>8</v>
       </c>
       <c r="L23" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M23" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N23" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O23" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P23" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q23" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R23" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" s="10">
         <v>1</v>
@@ -2589,25 +2655,25 @@
         <v>1</v>
       </c>
       <c r="O24" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="10">
         <v>1</v>
@@ -2643,27 +2709,29 @@
         <v>1</v>
       </c>
       <c r="O25" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R25" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>42</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="4">
+        <v>10</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -2679,13 +2747,13 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" ht="70">
+    <row r="27" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="9">
         <v>8</v>
@@ -2712,34 +2780,34 @@
         <v>8</v>
       </c>
       <c r="L27" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M27" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N27" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O27" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P27" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q27" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R27" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="10">
         <v>1</v>
@@ -2775,25 +2843,25 @@
         <v>1</v>
       </c>
       <c r="O28" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" s="10">
         <v>1</v>
@@ -2829,24 +2897,24 @@
         <v>1</v>
       </c>
       <c r="O29" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q29" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R29" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>41</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2865,13 +2933,13 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="70">
+    <row r="31" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="9">
         <v>8</v>
@@ -2898,34 +2966,34 @@
         <v>8</v>
       </c>
       <c r="L31" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M31" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N31" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O31" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P31" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q31" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R31" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" s="10">
         <v>1</v>
@@ -2961,25 +3029,25 @@
         <v>1</v>
       </c>
       <c r="O32" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R32" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D33" s="10">
         <v>1</v>
@@ -3015,24 +3083,24 @@
         <v>1</v>
       </c>
       <c r="O33" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q33" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>39</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -3051,13 +3119,13 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="70">
+    <row r="35" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D35" s="9">
         <v>8</v>
@@ -3084,34 +3152,34 @@
         <v>8</v>
       </c>
       <c r="L35" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M35" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N35" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O35" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P35" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q35" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R35" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D36" s="10">
         <v>1</v>
@@ -3147,25 +3215,25 @@
         <v>1</v>
       </c>
       <c r="O36" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P36" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q36" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R36" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D37" s="10">
         <v>1</v>
@@ -3201,27 +3269,29 @@
         <v>1</v>
       </c>
       <c r="O37" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P37" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q37" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R37" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
+      <c r="D38" s="4">
+        <v>10</v>
+      </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -3237,13 +3307,13 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" ht="70">
+    <row r="39" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" s="9">
         <v>8</v>
@@ -3270,34 +3340,34 @@
         <v>8</v>
       </c>
       <c r="L39" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M39" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N39" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O39" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P39" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q39" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R39" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="70">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D40" s="10">
         <v>1</v>
@@ -3333,25 +3403,25 @@
         <v>1</v>
       </c>
       <c r="O40" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P40" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q40" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D41" s="10">
         <v>1</v>
@@ -3387,27 +3457,29 @@
         <v>1</v>
       </c>
       <c r="O41" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P41" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q41" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R41" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>17</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="D42" s="4">
+        <v>10</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -3423,13 +3495,13 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D43" s="9">
         <v>8</v>
@@ -3456,34 +3528,34 @@
         <v>8</v>
       </c>
       <c r="L43" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M43" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N43" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O43" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P43" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q43" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R43" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D44" s="10">
         <v>1</v>
@@ -3519,25 +3591,25 @@
         <v>1</v>
       </c>
       <c r="O44" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P44" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q44" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R44" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D45" s="10">
         <v>1</v>
@@ -3573,27 +3645,29 @@
         <v>1</v>
       </c>
       <c r="O45" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P45" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q45" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R45" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>21</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
+      <c r="D46" s="4">
+        <v>10</v>
+      </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -3609,13 +3683,13 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D47" s="9">
         <v>8</v>
@@ -3642,34 +3716,34 @@
         <v>8</v>
       </c>
       <c r="L47" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M47" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N47" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O47" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P47" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q47" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R47" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D48" s="10">
         <v>1</v>
@@ -3705,25 +3779,25 @@
         <v>1</v>
       </c>
       <c r="O48" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P48" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q48" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D49" s="10">
         <v>1</v>
@@ -3759,27 +3833,29 @@
         <v>1</v>
       </c>
       <c r="O49" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P49" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q49" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R49" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>19</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
+      <c r="D50" s="4">
+        <v>10</v>
+      </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -3795,13 +3871,13 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="B51" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D51" s="9">
         <v>8</v>
@@ -3828,34 +3904,34 @@
         <v>8</v>
       </c>
       <c r="L51" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M51" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N51" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O51" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P51" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q51" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R51" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D52" s="10">
         <v>1</v>
@@ -3891,25 +3967,25 @@
         <v>1</v>
       </c>
       <c r="O52" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P52" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q52" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R52" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D53" s="10">
         <v>1</v>
@@ -3945,27 +4021,29 @@
         <v>1</v>
       </c>
       <c r="O53" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P53" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q53" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R53" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>18</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
+      <c r="D54" s="4">
+        <v>10</v>
+      </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -3981,13 +4059,13 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D55" s="9">
         <v>8</v>
@@ -4014,34 +4092,34 @@
         <v>8</v>
       </c>
       <c r="L55" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M55" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N55" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O55" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P55" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q55" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R55" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D56" s="10">
         <v>1</v>
@@ -4077,25 +4155,25 @@
         <v>1</v>
       </c>
       <c r="O56" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P56" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q56" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R56" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D57" s="10">
         <v>1</v>
@@ -4131,27 +4209,29 @@
         <v>1</v>
       </c>
       <c r="O57" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P57" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q57" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R57" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>20</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
+      <c r="D58" s="4">
+        <v>10</v>
+      </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -4167,13 +4247,13 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="B59" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D59" s="9">
         <v>8</v>
@@ -4200,34 +4280,34 @@
         <v>8</v>
       </c>
       <c r="L59" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M59" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N59" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O59" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P59" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q59" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R59" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D60" s="10">
         <v>1</v>
@@ -4263,25 +4343,25 @@
         <v>1</v>
       </c>
       <c r="O60" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P60" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q60" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R60" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D61" s="10">
         <v>1</v>
@@ -4317,27 +4397,29 @@
         <v>1</v>
       </c>
       <c r="O61" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P61" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q61" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R61" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>4</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
+      <c r="D62" s="4">
+        <v>10</v>
+      </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -4353,13 +4435,13 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="9"/>
       <c r="B63" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D63" s="9">
         <v>8</v>
@@ -4386,34 +4468,34 @@
         <v>8</v>
       </c>
       <c r="L63" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M63" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N63" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O63" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P63" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q63" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R63" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D64" s="10">
         <v>1</v>
@@ -4449,25 +4531,25 @@
         <v>1</v>
       </c>
       <c r="O64" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P64" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q64" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R64" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D65" s="10">
         <v>1</v>
@@ -4503,27 +4585,29 @@
         <v>1</v>
       </c>
       <c r="O65" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P65" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q65" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R65" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>25</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
+      <c r="D66" s="4">
+        <v>10</v>
+      </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
@@ -4539,13 +4623,13 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" spans="1:18" ht="28">
+    <row r="67" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="9"/>
       <c r="B67" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D67" s="9">
         <v>8</v>
@@ -4572,34 +4656,34 @@
         <v>8</v>
       </c>
       <c r="L67" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M67" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N67" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O67" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P67" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q67" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R67" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" ht="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D68" s="10">
         <v>1</v>
@@ -4635,25 +4719,25 @@
         <v>1</v>
       </c>
       <c r="O68" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P68" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q68" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R68" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D69" s="10">
         <v>1</v>
@@ -4689,27 +4773,29 @@
         <v>1</v>
       </c>
       <c r="O69" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P69" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q69" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R69" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>26</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
+      <c r="D70" s="4">
+        <v>10</v>
+      </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -4725,13 +4811,13 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" ht="28">
+    <row r="71" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="9"/>
       <c r="B71" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D71" s="9">
         <v>8</v>
@@ -4758,34 +4844,34 @@
         <v>8</v>
       </c>
       <c r="L71" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M71" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N71" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O71" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P71" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q71" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R71" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" ht="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D72" s="10">
         <v>1</v>
@@ -4821,25 +4907,25 @@
         <v>1</v>
       </c>
       <c r="O72" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P72" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q72" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R72" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D73" s="10">
         <v>1</v>
@@ -4875,27 +4961,29 @@
         <v>1</v>
       </c>
       <c r="O73" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P73" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q73" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R73" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>27</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
+      <c r="D74" s="4">
+        <v>10</v>
+      </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -4911,13 +4999,13 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" ht="28">
+    <row r="75" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="9"/>
       <c r="B75" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D75" s="9">
         <v>8</v>
@@ -4944,34 +5032,34 @@
         <v>8</v>
       </c>
       <c r="L75" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M75" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N75" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O75" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P75" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q75" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R75" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" ht="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D76" s="10">
         <v>1</v>
@@ -5007,25 +5095,25 @@
         <v>1</v>
       </c>
       <c r="O76" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P76" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q76" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R76" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
       <c r="B77" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D77" s="10">
         <v>1</v>
@@ -5061,27 +5149,29 @@
         <v>1</v>
       </c>
       <c r="O77" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P77" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q77" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R77" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>29</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
+      <c r="D78" s="4">
+        <v>10</v>
+      </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -5097,13 +5187,13 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" ht="28">
+    <row r="79" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="9"/>
       <c r="B79" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D79" s="9">
         <v>8</v>
@@ -5130,34 +5220,34 @@
         <v>8</v>
       </c>
       <c r="L79" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M79" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N79" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O79" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P79" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q79" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R79" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" ht="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D80" s="10">
         <v>1</v>
@@ -5193,25 +5283,25 @@
         <v>1</v>
       </c>
       <c r="O80" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P80" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q80" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R80" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D81" s="10">
         <v>1</v>
@@ -5247,27 +5337,29 @@
         <v>1</v>
       </c>
       <c r="O81" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P81" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q81" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R81" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>30</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
+      <c r="D82" s="4">
+        <v>10</v>
+      </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -5283,13 +5375,13 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" ht="28">
+    <row r="83" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="9"/>
       <c r="B83" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D83" s="9">
         <v>8</v>
@@ -5316,34 +5408,34 @@
         <v>8</v>
       </c>
       <c r="L83" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M83" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N83" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O83" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P83" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q83" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R83" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" ht="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="10"/>
       <c r="B84" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D84" s="10">
         <v>1</v>
@@ -5379,25 +5471,25 @@
         <v>1</v>
       </c>
       <c r="O84" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P84" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q84" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R84" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="B85" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D85" s="10">
         <v>1</v>
@@ -5433,27 +5525,29 @@
         <v>1</v>
       </c>
       <c r="O85" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P85" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q85" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R85" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>31</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
+      <c r="D86" s="4">
+        <v>10</v>
+      </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
@@ -5469,13 +5563,13 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18" ht="28">
+    <row r="87" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="9"/>
       <c r="B87" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D87" s="9">
         <v>8</v>
@@ -5502,34 +5596,34 @@
         <v>8</v>
       </c>
       <c r="L87" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M87" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N87" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O87" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P87" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q87" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R87" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" ht="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
       <c r="B88" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D88" s="10">
         <v>1</v>
@@ -5565,25 +5659,25 @@
         <v>1</v>
       </c>
       <c r="O88" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P88" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q88" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R88" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
       <c r="B89" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D89" s="10">
         <v>1</v>
@@ -5619,27 +5713,29 @@
         <v>1</v>
       </c>
       <c r="O89" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P89" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q89" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R89" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>33</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
+      <c r="D90" s="4">
+        <v>10</v>
+      </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
@@ -5655,13 +5751,13 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18" ht="28">
+    <row r="91" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="9"/>
       <c r="B91" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D91" s="9">
         <v>8</v>
@@ -5688,34 +5784,34 @@
         <v>8</v>
       </c>
       <c r="L91" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M91" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N91" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O91" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P91" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q91" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R91" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" ht="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="10"/>
       <c r="B92" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D92" s="10">
         <v>1</v>
@@ -5751,25 +5847,25 @@
         <v>1</v>
       </c>
       <c r="O92" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P92" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q92" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R92" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
       <c r="B93" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D93" s="10">
         <v>1</v>
@@ -5805,27 +5901,29 @@
         <v>1</v>
       </c>
       <c r="O93" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P93" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q93" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R93" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>22</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C94" s="4"/>
-      <c r="D94" s="4"/>
+      <c r="D94" s="4">
+        <v>10</v>
+      </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
@@ -5841,13 +5939,13 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="9"/>
       <c r="B95" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D95" s="9">
         <v>8</v>
@@ -5874,34 +5972,34 @@
         <v>8</v>
       </c>
       <c r="L95" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M95" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N95" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O95" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P95" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q95" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R95" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
       <c r="B96" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D96" s="10">
         <v>1</v>
@@ -5937,25 +6035,25 @@
         <v>1</v>
       </c>
       <c r="O96" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P96" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q96" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R96" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
       <c r="B97" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D97" s="10">
         <v>1</v>
@@ -5991,27 +6089,29 @@
         <v>1</v>
       </c>
       <c r="O97" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P97" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q97" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R97" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>35</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
+      <c r="D98" s="4">
+        <v>10</v>
+      </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
       <c r="G98" s="4"/>
@@ -6027,13 +6127,13 @@
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="9"/>
       <c r="B99" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D99" s="9">
         <v>8</v>
@@ -6060,34 +6160,34 @@
         <v>8</v>
       </c>
       <c r="L99" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M99" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N99" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O99" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P99" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q99" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R99" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
       <c r="B100" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D100" s="10">
         <v>1</v>
@@ -6123,25 +6223,25 @@
         <v>1</v>
       </c>
       <c r="O100" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P100" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q100" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R100" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
       <c r="B101" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D101" s="10">
         <v>1</v>
@@ -6177,27 +6277,29 @@
         <v>1</v>
       </c>
       <c r="O101" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P101" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q101" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R101" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" ht="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>24</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
+      <c r="D102" s="4">
+        <v>10</v>
+      </c>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
@@ -6213,13 +6315,13 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="9"/>
       <c r="B103" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D103" s="9">
         <v>8</v>
@@ -6246,34 +6348,34 @@
         <v>8</v>
       </c>
       <c r="L103" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M103" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N103" s="9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O103" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P103" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q103" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R103" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="10"/>
       <c r="B104" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D104" s="10">
         <v>1</v>
@@ -6309,25 +6411,25 @@
         <v>1</v>
       </c>
       <c r="O104" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P104" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q104" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R104" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
       <c r="B105" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D105" s="10">
         <v>1</v>
@@ -6363,16 +6465,16 @@
         <v>1</v>
       </c>
       <c r="O105" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P105" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q105" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R105" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6399,17 +6501,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A21:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="15" width="8.83203125" style="1"/>
+    <col min="2" max="15" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="5" t="s">
         <v>6</v>
@@ -6454,122 +6556,122 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="7" t="e">
+      <c r="B22" s="7">
         <f>'Sprint-Backlog'!E5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C22" s="7" t="e">
+        <v>20</v>
+      </c>
+      <c r="C22" s="7">
         <f>'Sprint-Backlog'!F5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D22" s="7" t="e">
+        <v>20</v>
+      </c>
+      <c r="D22" s="7">
         <f>'Sprint-Backlog'!G5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="E22" s="7">
         <f>'Sprint-Backlog'!H5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="F22" s="7">
         <f>'Sprint-Backlog'!I5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="G22" s="7">
         <f>'Sprint-Backlog'!J5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="H22" s="7">
         <f>'Sprint-Backlog'!K5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="I22" s="7">
         <f>'Sprint-Backlog'!L5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="J22" s="7">
         <f>'Sprint-Backlog'!M5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="K22" s="7">
         <f>'Sprint-Backlog'!N5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="L22" s="7">
         <f>'Sprint-Backlog'!O5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="M22" s="7">
         <f>'Sprint-Backlog'!P5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="N22" s="7">
         <f>'Sprint-Backlog'!Q5</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O22" s="7" t="e">
+        <v>19</v>
+      </c>
+      <c r="O22" s="7">
         <f>'Sprint-Backlog'!R5</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="7" t="e">
+      <c r="B23" s="7">
         <f>B22</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C23" s="7" t="e">
+        <v>20</v>
+      </c>
+      <c r="C23" s="7">
         <f t="shared" ref="C23:N23" si="0">ROUND(B23-($B$22/13),0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D23" s="7" t="e">
+        <v>18</v>
+      </c>
+      <c r="D23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E23" s="7" t="e">
+        <v>16</v>
+      </c>
+      <c r="E23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="F23" s="7" t="e">
+        <v>14</v>
+      </c>
+      <c r="F23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="G23" s="7" t="e">
+        <v>12</v>
+      </c>
+      <c r="G23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="H23" s="7" t="e">
+        <v>10</v>
+      </c>
+      <c r="H23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I23" s="7" t="e">
+        <v>8</v>
+      </c>
+      <c r="I23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="J23" s="7" t="e">
+        <v>6</v>
+      </c>
+      <c r="J23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="K23" s="7" t="e">
+        <v>4</v>
+      </c>
+      <c r="K23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="L23" s="7" t="e">
+        <v>2</v>
+      </c>
+      <c r="L23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="M23" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="M23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="N23" s="7" t="e">
+        <v>-2</v>
+      </c>
+      <c r="N23" s="7">
         <f t="shared" si="0"/>
-        <v>#REF!</v>
+        <v>-4</v>
       </c>
       <c r="O23" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
Elaboracao do relatorio de status da sprint 3 semana 6
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Sprint-Backlog-Sprint-03#.xlsx
+++ b/Trunk/Doc/Sprint-Backlog-Sprint-03#.xlsx
@@ -981,13 +981,13 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1186,11 +1186,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="6945344"/>
-        <c:axId val="6946432"/>
+        <c:axId val="-247670192"/>
+        <c:axId val="-247672368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6945344"/>
+        <c:axId val="-247670192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,7 +1210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6946432"/>
+        <c:crossAx val="-247672368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1218,7 +1218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6946432"/>
+        <c:axId val="-247672368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,7 +1245,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6945344"/>
+        <c:crossAx val="-247670192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1590,7 +1590,7 @@
   <dimension ref="A1:R105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:R7"/>
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,15 +1774,15 @@
       </c>
       <c r="P5" s="11">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="11">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="R5" s="11">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1856,13 +1856,13 @@
         <v>7</v>
       </c>
       <c r="P7" s="9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Q7" s="9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="R7" s="9">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -1913,10 +1913,10 @@
         <v>1</v>
       </c>
       <c r="Q8" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -2042,13 +2042,13 @@
         <v>8</v>
       </c>
       <c r="P11" s="9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R11" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -2099,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="Q12" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -2153,10 +2153,10 @@
         <v>1</v>
       </c>
       <c r="Q13" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -2233,10 +2233,10 @@
         <v>7</v>
       </c>
       <c r="Q15" s="9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="R15" s="9">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -2287,10 +2287,10 @@
         <v>1</v>
       </c>
       <c r="Q16" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -2969,22 +2969,22 @@
         <v>8</v>
       </c>
       <c r="M31" s="9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N31" s="9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O31" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P31" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R31" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -3026,19 +3026,19 @@
         <v>1</v>
       </c>
       <c r="N32" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R32" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -3083,16 +3083,16 @@
         <v>1</v>
       </c>
       <c r="O33" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P33" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R33" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -3158,19 +3158,19 @@
         <v>8</v>
       </c>
       <c r="N35" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O35" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P35" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R35" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -3212,19 +3212,19 @@
         <v>1</v>
       </c>
       <c r="N36" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O36" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P36" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R36" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -3266,19 +3266,19 @@
         <v>1</v>
       </c>
       <c r="N37" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O37" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P37" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R37" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -4668,13 +4668,13 @@
         <v>8</v>
       </c>
       <c r="P67" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q67" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R67" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -4722,13 +4722,13 @@
         <v>1</v>
       </c>
       <c r="P68" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q68" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R68" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -4776,13 +4776,13 @@
         <v>1</v>
       </c>
       <c r="P69" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q69" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R69" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -4856,13 +4856,13 @@
         <v>8</v>
       </c>
       <c r="P71" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q71" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R71" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -4913,10 +4913,10 @@
         <v>1</v>
       </c>
       <c r="Q72" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R72" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -4967,10 +4967,10 @@
         <v>1</v>
       </c>
       <c r="Q73" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R73" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -5044,13 +5044,13 @@
         <v>8</v>
       </c>
       <c r="P75" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q75" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="R75" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -5101,10 +5101,10 @@
         <v>1</v>
       </c>
       <c r="Q76" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R76" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -5155,10 +5155,10 @@
         <v>1</v>
       </c>
       <c r="Q77" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R77" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -5608,13 +5608,13 @@
         <v>8</v>
       </c>
       <c r="P87" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q87" s="9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R87" s="9">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -5665,10 +5665,10 @@
         <v>1</v>
       </c>
       <c r="Q88" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R88" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -5799,10 +5799,10 @@
         <v>8</v>
       </c>
       <c r="Q91" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="R91" s="9">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -5853,10 +5853,10 @@
         <v>1</v>
       </c>
       <c r="Q92" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R92" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -6095,7 +6095,7 @@
         <v>1</v>
       </c>
       <c r="Q97" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R97" s="10">
         <v>1</v>
@@ -6360,13 +6360,13 @@
         <v>8</v>
       </c>
       <c r="P103" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q103" s="9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="R103" s="9">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
@@ -6417,10 +6417,10 @@
         <v>1</v>
       </c>
       <c r="Q104" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R104" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
@@ -6501,7 +6501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A21:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -6606,15 +6606,15 @@
       </c>
       <c r="M22" s="7">
         <f>'Sprint-Backlog'!P5</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="N22" s="7">
         <f>'Sprint-Backlog'!Q5</f>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="O22" s="7">
         <f>'Sprint-Backlog'!R5</f>
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>